<commit_message>
Remove "keywords" from Performance model
</commit_message>
<xml_diff>
--- a/src/dye/testfiles/invalid_DOI.xlsx
+++ b/src/dye/testfiles/invalid_DOI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/Projects/solar/testfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/Projects/solar/src/dye/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>String</t>
   </si>
@@ -507,53 +507,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="97" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="97" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -596,25 +596,22 @@
       <c r="N9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="6" t="s">
+      <c r="O9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="P9" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="Q9" s="1">
+        <v>438</v>
+      </c>
       <c r="R9" s="1">
-        <v>438</v>
-      </c>
-      <c r="S9" s="1">
         <v>585</v>
       </c>
+      <c r="S9" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="T9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U9" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>